<commit_message>
chnge font alignment for excle
</commit_message>
<xml_diff>
--- a/日报模板.xlsx
+++ b/日报模板.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\host_check\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\host_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{23B71CA4-6A83-449D-ADC4-98DFDCB56EA9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12444" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="巡检明细" sheetId="4" r:id="rId1"/>
@@ -1158,7 +1159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.000%"/>
   </numFmts>
@@ -1676,9 +1677,6 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1807,6 +1805,77 @@
     <xf numFmtId="176" fontId="35" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1814,14 +1883,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1838,42 +1899,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1904,37 +1929,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规_巡检明细" xfId="1"/>
+    <cellStyle name="常规_巡检明细" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="99">
@@ -2859,7 +2860,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6500" name="图片 2"/>
+        <xdr:cNvPr id="6500" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000064190000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3201,61 +3208,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.8984375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="14.09765625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="26" customWidth="1"/>
     <col min="4" max="4" width="48.5" style="27" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="104" customWidth="1"/>
-    <col min="6" max="6" width="32.59765625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="15.8984375" style="26" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="70" customWidth="1"/>
+    <col min="6" max="6" width="32.625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="15.875" style="26" customWidth="1"/>
     <col min="8" max="8" width="9" style="26" customWidth="1"/>
     <col min="9" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="178.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="178.9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="89" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="67"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D2)),ISERROR(SEARCH("86%",D2)),ISERROR(SEARCH("87%",D2)),ISERROR(SEARCH("88%",D2)),ISERROR(SEARCH("89%",D2)),ISERROR(SEARCH("9?%",D2)),ISERROR(SEARCH("0?%",D2))),"正常","异常")</f>
         <v>正常</v>
@@ -3263,13 +3270,13 @@
       <c r="F2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="59" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71"/>
-      <c r="B3" s="73"/>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="88"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
@@ -3285,9 +3292,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="71"/>
-      <c r="B4" s="73"/>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="88"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -3303,13 +3310,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="73"/>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="88"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="7" t="str">
         <f>IF(D5&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3321,15 +3328,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="181.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="74" t="s">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="181.9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="88"/>
+      <c r="B6" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="67"/>
+      <c r="D6" s="66"/>
       <c r="E6" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D6)),ISERROR(SEARCH("86%",D6)),ISERROR(SEARCH("87%",D6)),ISERROR(SEARCH("88%",D6)),ISERROR(SEARCH("89%",D6)),ISERROR(SEARCH("9?%",D6)),ISERROR(SEARCH("0?%",D6))),"正常","异常")</f>
         <v>正常</v>
@@ -3341,9 +3348,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="73"/>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="88"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
@@ -3359,9 +3366,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73"/>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="88"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
@@ -3377,13 +3384,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="73"/>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="88"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="7" t="str">
         <f>IF(D9&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3395,15 +3402,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="73" t="s">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="88"/>
+      <c r="B10" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="67"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D10)),ISERROR(SEARCH("86%",D10)),ISERROR(SEARCH("87%",D10)),ISERROR(SEARCH("88%",D10)),ISERROR(SEARCH("89%",D10)),ISERROR(SEARCH("9?%",D10)),ISERROR(SEARCH("0?%",D10))),"正常","异常")</f>
         <v>正常</v>
@@ -3415,9 +3422,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="73"/>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="88"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
@@ -3433,9 +3440,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="73"/>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="88"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -3451,13 +3458,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="73"/>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="88"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="31"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="7" t="str">
         <f>IF(D13&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3469,15 +3476,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="184.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
-      <c r="B14" s="75" t="s">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="184.9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="88"/>
+      <c r="B14" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="67"/>
+      <c r="D14" s="66"/>
       <c r="E14" s="7" t="s">
         <v>20</v>
       </c>
@@ -3488,9 +3495,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="73"/>
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="88"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
@@ -3506,9 +3513,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="73"/>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="88"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
@@ -3524,13 +3531,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="73"/>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="88"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="7" t="str">
         <f>IF(D17&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3542,15 +3549,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="73" t="s">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="88"/>
+      <c r="B18" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="67"/>
+      <c r="D18" s="66"/>
       <c r="E18" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D18)),ISERROR(SEARCH("86%",D18)),ISERROR(SEARCH("87%",D18)),ISERROR(SEARCH("88%",D18)),ISERROR(SEARCH("89%",D18)),ISERROR(SEARCH("9?%",D18)),ISERROR(SEARCH("0?%",D18))),"正常","异常")</f>
         <v>正常</v>
@@ -3562,10 +3569,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="68" t="s">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="88"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="67" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="6"/>
@@ -3580,9 +3587,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="73"/>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="88"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="5" t="s">
         <v>13</v>
       </c>
@@ -3598,13 +3605,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
-      <c r="B21" s="73"/>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="88"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="31"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="7" t="str">
         <f>IF(D21&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3616,15 +3623,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="73" t="s">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="156.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="88"/>
+      <c r="B22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="67"/>
+      <c r="D22" s="66"/>
       <c r="E22" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D22)),ISERROR(SEARCH("86%",D22)),ISERROR(SEARCH("87%",D22)),ISERROR(SEARCH("88%",D22)),ISERROR(SEARCH("89%",D22)),ISERROR(SEARCH("9?%",D22)),ISERROR(SEARCH("0?%",D22))),"正常","异常")</f>
         <v>正常</v>
@@ -3636,9 +3643,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="73"/>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="88"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="5" t="s">
         <v>10</v>
       </c>
@@ -3654,9 +3661,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
-      <c r="B24" s="73"/>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="88"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="5" t="s">
         <v>13</v>
       </c>
@@ -3672,13 +3679,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="73"/>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="88"/>
+      <c r="B25" s="72"/>
       <c r="C25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="31"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="7" t="str">
         <f>IF(D25&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3690,15 +3697,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="177.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="73" t="s">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="177.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="88"/>
+      <c r="B26" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="67"/>
+      <c r="D26" s="66"/>
       <c r="E26" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D26)),ISERROR(SEARCH("86%",D26)),ISERROR(SEARCH("87%",D26)),ISERROR(SEARCH("88%",D26)),ISERROR(SEARCH("89%",D26)),ISERROR(SEARCH("9?%",D26)),ISERROR(SEARCH("0?%",D26))),"正常","异常")</f>
         <v>正常</v>
@@ -3710,9 +3717,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="73"/>
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="88"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="5" t="s">
         <v>10</v>
       </c>
@@ -3728,9 +3735,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="71"/>
-      <c r="B28" s="73"/>
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="88"/>
+      <c r="B28" s="72"/>
       <c r="C28" s="5" t="s">
         <v>13</v>
       </c>
@@ -3746,13 +3753,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="71"/>
-      <c r="B29" s="73"/>
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="88"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="31"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="7" t="str">
         <f>IF(D29&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3764,15 +3771,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="176.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
-      <c r="B30" s="78" t="s">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="176.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="88"/>
+      <c r="B30" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="67"/>
+      <c r="D30" s="66"/>
       <c r="E30" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D30)),ISERROR(SEARCH("86%",D30)),ISERROR(SEARCH("87%",D30)),ISERROR(SEARCH("88%",D30)),ISERROR(SEARCH("89%",D30)),ISERROR(SEARCH("9?%",D30)),ISERROR(SEARCH("0?%",D30))),"正常","异常")</f>
         <v>正常</v>
@@ -3784,9 +3791,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
-      <c r="B31" s="73"/>
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="88"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="5" t="s">
         <v>10</v>
       </c>
@@ -3802,10 +3809,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="47" t="s">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="88"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="46" t="s">
         <v>117</v>
       </c>
       <c r="D32" s="6"/>
@@ -3820,13 +3827,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="71"/>
-      <c r="B33" s="73"/>
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="88"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="31"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="7" t="str">
         <f>IF(D33&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3838,15 +3845,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="71"/>
-      <c r="B34" s="73" t="s">
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="88"/>
+      <c r="B34" s="72" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="67"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D34)),ISERROR(SEARCH("86%",D34)),ISERROR(SEARCH("87%",D34)),ISERROR(SEARCH("88%",D34)),ISERROR(SEARCH("89%",D34)),ISERROR(SEARCH("9?%",D34)),ISERROR(SEARCH("0?%",D34))),"正常","异常")</f>
         <v>正常</v>
@@ -3858,9 +3865,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
-      <c r="B35" s="73"/>
+    <row r="35" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="88"/>
+      <c r="B35" s="72"/>
       <c r="C35" s="5" t="s">
         <v>10</v>
       </c>
@@ -3876,9 +3883,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
-      <c r="B36" s="73"/>
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="88"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="5" t="s">
         <v>13</v>
       </c>
@@ -3894,13 +3901,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
-      <c r="B37" s="73"/>
+    <row r="37" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="88"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="31"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="7" t="str">
         <f>IF(D37&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3912,15 +3919,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
-      <c r="B38" s="73" t="s">
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="88"/>
+      <c r="B38" s="72" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D38" s="67"/>
+      <c r="D38" s="66"/>
       <c r="E38" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D38)),ISERROR(SEARCH("86%",D38)),ISERROR(SEARCH("87%",D38)),ISERROR(SEARCH("88%",D38)),ISERROR(SEARCH("89%",D38)),ISERROR(SEARCH("9?%",D38)),ISERROR(SEARCH("0?%",D38))),"正常","异常")</f>
         <v>正常</v>
@@ -3932,10 +3939,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="53" t="s">
+    <row r="39" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="88"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="52" t="s">
         <v>113</v>
       </c>
       <c r="D39" s="6"/>
@@ -3950,10 +3957,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="71"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="54" t="s">
+    <row r="40" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="88"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="53" t="s">
         <v>136</v>
       </c>
       <c r="D40" s="6"/>
@@ -3968,13 +3975,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="71"/>
-      <c r="B41" s="73"/>
+    <row r="41" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="88"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="31"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="7" t="str">
         <f>IF(D41&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -3986,15 +3993,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="71"/>
-      <c r="B42" s="79" t="s">
+    <row r="42" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="88"/>
+      <c r="B42" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="67"/>
+      <c r="D42" s="66"/>
       <c r="E42" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D42)),ISERROR(SEARCH("86%",D42)),ISERROR(SEARCH("87%",D42)),ISERROR(SEARCH("88%",D42)),ISERROR(SEARCH("89%",D42)),ISERROR(SEARCH("9?%",D42)),ISERROR(SEARCH("0?%",D42))),"正常","异常")</f>
         <v>正常</v>
@@ -4006,10 +4013,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="80"/>
-      <c r="C43" s="44" t="s">
+    <row r="43" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="88"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="43" t="s">
         <v>113</v>
       </c>
       <c r="D43" s="6"/>
@@ -4024,10 +4031,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="80"/>
-      <c r="C44" s="55" t="s">
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="88"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="54" t="s">
         <v>107</v>
       </c>
       <c r="D44" s="6"/>
@@ -4042,13 +4049,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="71"/>
-      <c r="B45" s="80"/>
+    <row r="45" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="88"/>
+      <c r="B45" s="84"/>
       <c r="C45" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="31"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="7" t="str">
         <f>IF(D45&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4060,15 +4067,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="71"/>
-      <c r="B46" s="79" t="s">
+    <row r="46" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="88"/>
+      <c r="B46" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="67"/>
+      <c r="D46" s="66"/>
       <c r="E46" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D46)),ISERROR(SEARCH("86%",D46)),ISERROR(SEARCH("87%",D46)),ISERROR(SEARCH("88%",D46)),ISERROR(SEARCH("89%",D46)),ISERROR(SEARCH("9?%",D46)),ISERROR(SEARCH("0?%",D46))),"正常","异常")</f>
         <v>正常</v>
@@ -4080,9 +4087,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
-      <c r="B47" s="80"/>
+    <row r="47" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="88"/>
+      <c r="B47" s="84"/>
       <c r="C47" s="5" t="s">
         <v>10</v>
       </c>
@@ -4098,9 +4105,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="71"/>
-      <c r="B48" s="80"/>
+    <row r="48" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="88"/>
+      <c r="B48" s="84"/>
       <c r="C48" s="5" t="s">
         <v>121</v>
       </c>
@@ -4116,13 +4123,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="71"/>
-      <c r="B49" s="80"/>
+    <row r="49" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="88"/>
+      <c r="B49" s="84"/>
       <c r="C49" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="31"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="7" t="str">
         <f>IF(D49&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4134,15 +4141,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="71"/>
-      <c r="B50" s="79" t="s">
+    <row r="50" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="88"/>
+      <c r="B50" s="83" t="s">
         <v>28</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D50" s="67"/>
+      <c r="D50" s="66"/>
       <c r="E50" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D50)),ISERROR(SEARCH("86%",D50)),ISERROR(SEARCH("87%",D50)),ISERROR(SEARCH("88%",D50)),ISERROR(SEARCH("89%",D50)),ISERROR(SEARCH("9?%",D50)),ISERROR(SEARCH("0?%",D50))),"正常","异常")</f>
         <v>正常</v>
@@ -4154,9 +4161,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="71"/>
-      <c r="B51" s="80"/>
+    <row r="51" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="88"/>
+      <c r="B51" s="84"/>
       <c r="C51" s="5" t="s">
         <v>133</v>
       </c>
@@ -4172,9 +4179,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="71"/>
-      <c r="B52" s="80"/>
+    <row r="52" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="88"/>
+      <c r="B52" s="84"/>
       <c r="C52" s="5" t="s">
         <v>13</v>
       </c>
@@ -4190,13 +4197,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="71"/>
-      <c r="B53" s="80"/>
+    <row r="53" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="88"/>
+      <c r="B53" s="84"/>
       <c r="C53" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="31"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="7" t="str">
         <f>IF(D53&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4208,15 +4215,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="71"/>
-      <c r="B54" s="81" t="s">
+    <row r="54" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="88"/>
+      <c r="B54" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="67"/>
+      <c r="D54" s="66"/>
       <c r="E54" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D54)),ISERROR(SEARCH("86%",D54)),ISERROR(SEARCH("87%",D54)),ISERROR(SEARCH("88%",D54)),ISERROR(SEARCH("89%",D54)),ISERROR(SEARCH("9?%",D54)),ISERROR(SEARCH("0?%",D54))),"正常","异常")</f>
         <v>正常</v>
@@ -4228,10 +4235,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="71"/>
-      <c r="B55" s="82"/>
-      <c r="C55" s="51" t="s">
+    <row r="55" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="88"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="50" t="s">
         <v>124</v>
       </c>
       <c r="D55" s="6"/>
@@ -4246,9 +4253,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="71"/>
-      <c r="B56" s="82"/>
+    <row r="56" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="88"/>
+      <c r="B56" s="86"/>
       <c r="C56" s="5" t="s">
         <v>13</v>
       </c>
@@ -4264,13 +4271,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="71"/>
-      <c r="B57" s="83"/>
+    <row r="57" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="88"/>
+      <c r="B57" s="87"/>
       <c r="C57" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="31"/>
+      <c r="D57" s="30"/>
       <c r="E57" s="7" t="str">
         <f>IF(D57&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4282,15 +4289,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="71"/>
-      <c r="B58" s="73" t="s">
+    <row r="58" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="88"/>
+      <c r="B58" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="56" t="s">
+      <c r="C58" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D58" s="67"/>
+      <c r="D58" s="66"/>
       <c r="E58" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D58)),ISERROR(SEARCH("86%",D58)),ISERROR(SEARCH("87%",D58)),ISERROR(SEARCH("88%",D58)),ISERROR(SEARCH("89%",D58)),ISERROR(SEARCH("9?%",D58)),ISERROR(SEARCH("0?%",D58))),"正常","异常")</f>
         <v>正常</v>
@@ -4302,9 +4309,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="71"/>
-      <c r="B59" s="73"/>
+    <row r="59" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="88"/>
+      <c r="B59" s="72"/>
       <c r="C59" s="5" t="s">
         <v>113</v>
       </c>
@@ -4320,10 +4327,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="71"/>
-      <c r="B60" s="73"/>
-      <c r="C60" s="54" t="s">
+    <row r="60" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="88"/>
+      <c r="B60" s="72"/>
+      <c r="C60" s="53" t="s">
         <v>107</v>
       </c>
       <c r="D60" s="6"/>
@@ -4338,13 +4345,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="71"/>
-      <c r="B61" s="73"/>
+    <row r="61" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="88"/>
+      <c r="B61" s="72"/>
       <c r="C61" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="31"/>
+      <c r="D61" s="30"/>
       <c r="E61" s="7" t="str">
         <f>IF(D61&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4356,15 +4363,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="71"/>
-      <c r="B62" s="73" t="s">
+    <row r="62" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="88"/>
+      <c r="B62" s="72" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D62" s="67"/>
+      <c r="D62" s="66"/>
       <c r="E62" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D62)),ISERROR(SEARCH("86%",D62)),ISERROR(SEARCH("87%",D62)),ISERROR(SEARCH("88%",D62)),ISERROR(SEARCH("89%",D62)),ISERROR(SEARCH("9?%",D62)),ISERROR(SEARCH("0?%",D62))),"正常","异常")</f>
         <v>正常</v>
@@ -4376,9 +4383,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="71"/>
-      <c r="B63" s="73"/>
+    <row r="63" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="88"/>
+      <c r="B63" s="72"/>
       <c r="C63" s="5" t="s">
         <v>10</v>
       </c>
@@ -4394,9 +4401,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="71"/>
-      <c r="B64" s="73"/>
+    <row r="64" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="88"/>
+      <c r="B64" s="72"/>
       <c r="C64" s="5" t="s">
         <v>13</v>
       </c>
@@ -4412,13 +4419,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="71"/>
-      <c r="B65" s="73"/>
+    <row r="65" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="88"/>
+      <c r="B65" s="72"/>
       <c r="C65" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="31"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="7" t="str">
         <f>IF(D65&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4430,15 +4437,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="71"/>
-      <c r="B66" s="73" t="s">
+    <row r="66" spans="1:7" s="1" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="88"/>
+      <c r="B66" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="52" t="s">
+      <c r="C66" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="D66" s="67"/>
+      <c r="D66" s="66"/>
       <c r="E66" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D66)),ISERROR(SEARCH("86%",D66)),ISERROR(SEARCH("87%",D66)),ISERROR(SEARCH("88%",D66)),ISERROR(SEARCH("89%",D66)),ISERROR(SEARCH("9?%",D66)),ISERROR(SEARCH("0?%",D66))),"正常","异常")</f>
         <v>正常</v>
@@ -4450,9 +4457,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="71"/>
-      <c r="B67" s="73"/>
+    <row r="67" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="88"/>
+      <c r="B67" s="72"/>
       <c r="C67" s="5" t="s">
         <v>113</v>
       </c>
@@ -4468,10 +4475,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="71"/>
-      <c r="B68" s="73"/>
-      <c r="C68" s="52" t="s">
+    <row r="68" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="88"/>
+      <c r="B68" s="72"/>
+      <c r="C68" s="51" t="s">
         <v>107</v>
       </c>
       <c r="D68" s="6"/>
@@ -4486,13 +4493,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="71"/>
-      <c r="B69" s="73"/>
+    <row r="69" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="88"/>
+      <c r="B69" s="72"/>
       <c r="C69" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D69" s="31"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="7" t="str">
         <f>IF(D69&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4504,15 +4511,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A70" s="71"/>
-      <c r="B70" s="84" t="s">
+    <row r="70" spans="1:7" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="A70" s="88"/>
+      <c r="B70" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="64" t="s">
+      <c r="C70" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D70" s="67"/>
+      <c r="D70" s="66"/>
       <c r="E70" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D70)),ISERROR(SEARCH("86%",D70)),ISERROR(SEARCH("87%",D70)),ISERROR(SEARCH("88%",D70)),ISERROR(SEARCH("89%",D70)),ISERROR(SEARCH("9?%",D70)),ISERROR(SEARCH("0?%",D70))),"正常","异常")</f>
         <v>正常</v>
@@ -4524,13 +4531,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="71"/>
-      <c r="B71" s="73"/>
+    <row r="71" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="88"/>
+      <c r="B71" s="72"/>
       <c r="C71" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="43"/>
+      <c r="D71" s="42"/>
       <c r="E71" s="7" t="str">
         <f>IF(D71&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4542,9 +4549,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="71"/>
-      <c r="B72" s="73"/>
+    <row r="72" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="88"/>
+      <c r="B72" s="72"/>
       <c r="C72" s="5" t="s">
         <v>13</v>
       </c>
@@ -4560,13 +4567,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="71"/>
-      <c r="B73" s="73"/>
+    <row r="73" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="88"/>
+      <c r="B73" s="72"/>
       <c r="C73" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D73" s="31"/>
+      <c r="D73" s="30"/>
       <c r="E73" s="7" t="str">
         <f>IF(D73&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4578,15 +4585,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="1" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="71"/>
-      <c r="B74" s="76" t="s">
+    <row r="74" spans="1:7" s="1" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="88"/>
+      <c r="B74" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="57" t="s">
+      <c r="C74" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="69"/>
+      <c r="D74" s="68"/>
       <c r="E74" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D74)),ISERROR(SEARCH("86%",D74)),ISERROR(SEARCH("87%",D74)),ISERROR(SEARCH("88%",D74)),ISERROR(SEARCH("89%",D74)),ISERROR(SEARCH("9?%",D74)),ISERROR(SEARCH("0?%",D74))),"正常","异常")</f>
         <v>正常</v>
@@ -4598,13 +4605,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="71"/>
-      <c r="B75" s="77"/>
-      <c r="C75" s="32" t="s">
+    <row r="75" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="88"/>
+      <c r="B75" s="92"/>
+      <c r="C75" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="33"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="7" t="str">
         <f>IF(D75&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4616,13 +4623,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="71"/>
-      <c r="B76" s="77"/>
-      <c r="C76" s="32" t="s">
+    <row r="76" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="88"/>
+      <c r="B76" s="92"/>
+      <c r="C76" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D76" s="33"/>
+      <c r="D76" s="32"/>
       <c r="E76" s="7" t="str">
         <f>IF(D76&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4634,13 +4641,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="71"/>
-      <c r="B77" s="77"/>
-      <c r="C77" s="32" t="s">
+    <row r="77" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="88"/>
+      <c r="B77" s="92"/>
+      <c r="C77" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D77" s="34"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="7" t="str">
         <f>IF(D77&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4652,15 +4659,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="1" customFormat="1" ht="118.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="71"/>
-      <c r="B78" s="74" t="s">
+    <row r="78" spans="1:7" s="1" customFormat="1" ht="118.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="88"/>
+      <c r="B78" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="C78" s="53" t="s">
+      <c r="C78" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="67"/>
+      <c r="D78" s="66"/>
       <c r="E78" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D78)),ISERROR(SEARCH("86%",D78)),ISERROR(SEARCH("87%",D78)),ISERROR(SEARCH("88%",D78)),ISERROR(SEARCH("89%",D78)),ISERROR(SEARCH("9?%",D78)),ISERROR(SEARCH("0?%",D78))),"正常","异常")</f>
         <v>正常</v>
@@ -4672,9 +4679,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="71"/>
-      <c r="B79" s="73"/>
+    <row r="79" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="88"/>
+      <c r="B79" s="72"/>
       <c r="C79" s="5" t="s">
         <v>113</v>
       </c>
@@ -4690,9 +4697,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="71"/>
-      <c r="B80" s="73"/>
+    <row r="80" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="88"/>
+      <c r="B80" s="72"/>
       <c r="C80" s="5" t="s">
         <v>13</v>
       </c>
@@ -4708,13 +4715,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="71"/>
-      <c r="B81" s="73"/>
+    <row r="81" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="88"/>
+      <c r="B81" s="72"/>
       <c r="C81" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D81" s="31"/>
+      <c r="D81" s="30"/>
       <c r="E81" s="7" t="str">
         <f>IF(D81&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4726,15 +4733,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="1" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="71"/>
-      <c r="B82" s="87" t="s">
+    <row r="82" spans="1:7" s="1" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="88"/>
+      <c r="B82" s="79" t="s">
         <v>131</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D82" s="67"/>
+      <c r="D82" s="66"/>
       <c r="E82" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D82)),ISERROR(SEARCH("86%",D82)),ISERROR(SEARCH("87%",D82)),ISERROR(SEARCH("88%",D82)),ISERROR(SEARCH("89%",D82)),ISERROR(SEARCH("9?%",D82)),ISERROR(SEARCH("0?%",D82))),"正常","异常")</f>
         <v>正常</v>
@@ -4746,9 +4753,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="71"/>
-      <c r="B83" s="73"/>
+    <row r="83" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="88"/>
+      <c r="B83" s="72"/>
       <c r="C83" s="5" t="s">
         <v>139</v>
       </c>
@@ -4764,9 +4771,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="71"/>
-      <c r="B84" s="73"/>
+    <row r="84" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="88"/>
+      <c r="B84" s="72"/>
       <c r="C84" s="5" t="s">
         <v>122</v>
       </c>
@@ -4782,13 +4789,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="71"/>
-      <c r="B85" s="73"/>
+    <row r="85" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="88"/>
+      <c r="B85" s="72"/>
       <c r="C85" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D85" s="31"/>
+      <c r="D85" s="30"/>
       <c r="E85" s="7" t="str">
         <f>IF(D85&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4800,15 +4807,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A86" s="71"/>
-      <c r="B86" s="74" t="s">
+    <row r="86" spans="1:7" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="A86" s="88"/>
+      <c r="B86" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C86" s="64" t="s">
+      <c r="C86" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D86" s="70"/>
+      <c r="D86" s="69"/>
       <c r="E86" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D86)),ISERROR(SEARCH("86%",D86)),ISERROR(SEARCH("87%",D86)),ISERROR(SEARCH("88%",D86)),ISERROR(SEARCH("89%",D86)),ISERROR(SEARCH("9?%",D86)),ISERROR(SEARCH("0?%",D86))),"正常","异常")</f>
         <v>正常</v>
@@ -4820,13 +4827,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="71"/>
-      <c r="B87" s="73"/>
+    <row r="87" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="88"/>
+      <c r="B87" s="72"/>
       <c r="C87" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D87" s="31"/>
+      <c r="D87" s="30"/>
       <c r="E87" s="7" t="str">
         <f>IF(D87&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4838,13 +4845,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="71"/>
-      <c r="B88" s="73"/>
+    <row r="88" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="88"/>
+      <c r="B88" s="72"/>
       <c r="C88" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D88" s="31"/>
+      <c r="D88" s="30"/>
       <c r="E88" s="7" t="str">
         <f>IF(D88&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4856,13 +4863,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="71"/>
-      <c r="B89" s="73"/>
+    <row r="89" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="88"/>
+      <c r="B89" s="72"/>
       <c r="C89" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D89" s="31"/>
+      <c r="D89" s="30"/>
       <c r="E89" s="7" t="str">
         <f>IF(D89&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4874,15 +4881,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="1" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="71"/>
-      <c r="B90" s="74" t="s">
+    <row r="90" spans="1:7" s="1" customFormat="1" ht="112.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="88"/>
+      <c r="B90" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="53" t="s">
+      <c r="C90" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="D90" s="70"/>
+      <c r="D90" s="69"/>
       <c r="E90" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D90)),ISERROR(SEARCH("86%",D90)),ISERROR(SEARCH("87%",D90)),ISERROR(SEARCH("88%",D90)),ISERROR(SEARCH("89%",D90)),ISERROR(SEARCH("9?%",D90)),ISERROR(SEARCH("0?%",D90))),"正常","异常")</f>
         <v>正常</v>
@@ -4894,13 +4901,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="71"/>
-      <c r="B91" s="73"/>
+    <row r="91" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="88"/>
+      <c r="B91" s="72"/>
       <c r="C91" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D91" s="59"/>
+      <c r="D91" s="58"/>
       <c r="E91" s="7" t="str">
         <f>IF(D91&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4912,13 +4919,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="71"/>
-      <c r="B92" s="73"/>
+    <row r="92" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="88"/>
+      <c r="B92" s="72"/>
       <c r="C92" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D92" s="31"/>
+      <c r="D92" s="30"/>
       <c r="E92" s="7" t="str">
         <f>IF(D92&lt;85%,"正常","异常")</f>
         <v>正常</v>
@@ -4930,13 +4937,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="71"/>
-      <c r="B93" s="73"/>
-      <c r="C93" s="42" t="s">
+    <row r="93" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="88"/>
+      <c r="B93" s="72"/>
+      <c r="C93" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="D93" s="31"/>
+      <c r="D93" s="30"/>
       <c r="E93" s="7" t="str">
         <f>IF(D93&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -4948,15 +4955,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="1" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="71"/>
-      <c r="B94" s="74" t="s">
+    <row r="94" spans="1:7" s="1" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="88"/>
+      <c r="B94" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C94" s="66" t="s">
+      <c r="C94" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="D94" s="67"/>
+      <c r="D94" s="66"/>
       <c r="E94" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85%",D94)),ISERROR(SEARCH("86%",D94)),ISERROR(SEARCH("87%",D94)),ISERROR(SEARCH("88%",D94)),ISERROR(SEARCH("89%",D94)),ISERROR(SEARCH("9?%",D94)),ISERROR(SEARCH("0?%",D94))),"正常","异常")</f>
         <v>正常</v>
@@ -4968,9 +4975,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="71"/>
-      <c r="B95" s="73"/>
+    <row r="95" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="88"/>
+      <c r="B95" s="72"/>
       <c r="C95" s="5" t="s">
         <v>10</v>
       </c>
@@ -4986,9 +4993,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="71"/>
-      <c r="B96" s="73"/>
+    <row r="96" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="88"/>
+      <c r="B96" s="72"/>
       <c r="C96" s="5" t="s">
         <v>13</v>
       </c>
@@ -5004,13 +5011,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="71"/>
-      <c r="B97" s="73"/>
+    <row r="97" spans="1:7" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="88"/>
+      <c r="B97" s="72"/>
       <c r="C97" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D97" s="31"/>
+      <c r="D97" s="30"/>
       <c r="E97" s="7" t="str">
         <f>IF(D97&lt;5%,"正常","异常")</f>
         <v>正常</v>
@@ -5022,11 +5029,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="71" t="s">
+    <row r="98" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="B98" s="101" t="s">
+      <c r="B98" s="80" t="s">
         <v>38</v>
       </c>
       <c r="C98" s="5" t="s">
@@ -5044,13 +5051,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="71"/>
-      <c r="B99" s="102"/>
-      <c r="C99" s="63" t="s">
+    <row r="99" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="88"/>
+      <c r="B99" s="81"/>
+      <c r="C99" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="D99" s="65"/>
+      <c r="D99" s="64"/>
       <c r="E99" s="7" t="str">
         <f>IF(ISERROR(SEARCH("norowsselected",D99)),"异常","正常")</f>
         <v>异常</v>
@@ -5062,13 +5069,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="71"/>
-      <c r="B100" s="102"/>
-      <c r="C100" s="68" t="s">
+    <row r="100" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="88"/>
+      <c r="B100" s="81"/>
+      <c r="C100" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="D100" s="67"/>
+      <c r="D100" s="66"/>
       <c r="E100" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85.",D100)),ISERROR(SEARCH("86.",D100)),ISERROR(SEARCH("87.",D100)),ISERROR(SEARCH("88.",D100)),ISERROR(SEARCH("89.",D100)),ISERROR(SEARCH("9?.",D100)),ISERROR(SEARCH("100",D100))),"正常","异常")</f>
         <v>正常</v>
@@ -5080,33 +5087,33 @@
         <v>47</v>
       </c>
     </row>
-    <row r="101" spans="1:7" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="71"/>
-      <c r="B101" s="103"/>
+    <row r="101" spans="1:7" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="88"/>
+      <c r="B101" s="82"/>
       <c r="C101" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D101" s="67"/>
+      <c r="D101" s="66"/>
       <c r="E101" s="7" t="str">
         <f>IF(ISERROR(SEARCH("isnotnormal",D101)),"正常","异常")</f>
         <v>正常</v>
       </c>
-      <c r="F101" s="35" t="s">
+      <c r="F101" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="G101" s="36" t="s">
+      <c r="G101" s="35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:7" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="71"/>
-      <c r="B102" s="98" t="s">
+    <row r="102" spans="1:7" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="88"/>
+      <c r="B102" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="C102" s="66" t="s">
+      <c r="C102" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="D102" s="67"/>
+      <c r="D102" s="66"/>
       <c r="E102" s="7" t="str">
         <f>IF(ISERROR(SEARCH("norowsselected",D102)),"异常","正常")</f>
         <v>异常</v>
@@ -5118,13 +5125,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="103" spans="1:7" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="71"/>
-      <c r="B103" s="99"/>
-      <c r="C103" s="49" t="s">
+    <row r="103" spans="1:7" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="88"/>
+      <c r="B103" s="74"/>
+      <c r="C103" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="D103" s="65"/>
+      <c r="D103" s="64"/>
       <c r="E103" s="7" t="str">
         <f>IF(ISERROR(SEARCH("norowsselected",D103)),"异常","正常")</f>
         <v>异常</v>
@@ -5136,13 +5143,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:7" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="71"/>
-      <c r="B104" s="99"/>
-      <c r="C104" s="48" t="s">
+    <row r="104" spans="1:7" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="88"/>
+      <c r="B104" s="74"/>
+      <c r="C104" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="D104" s="67"/>
+      <c r="D104" s="66"/>
       <c r="E104" s="7" t="str">
         <f>IF(AND(ISERROR(SEARCH("85.",D104)),ISERROR(SEARCH("86.",D104)),ISERROR(SEARCH("87.",D104)),ISERROR(SEARCH("88.",D104)),ISERROR(SEARCH("89.",D104)),ISERROR(SEARCH("9?.",D104)),ISERROR(SEARCH("100",D104))),"正常","异常")</f>
         <v>正常</v>
@@ -5154,13 +5161,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="23" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="71"/>
-      <c r="B105" s="100"/>
+    <row r="105" spans="1:7" s="23" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="88"/>
+      <c r="B105" s="75"/>
       <c r="C105" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D105" s="67"/>
+      <c r="D105" s="66"/>
       <c r="E105" s="7" t="str">
         <f>IF(COUNTIF(D105,"*isnotnormal*"),"异常","正常")</f>
         <v>正常</v>
@@ -5172,12 +5179,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="4"/>
-      <c r="B106" s="86" t="s">
+      <c r="B106" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="C106" s="31" t="s">
         <v>56</v>
       </c>
       <c r="D106" s="6"/>
@@ -5192,10 +5199,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="4"/>
-      <c r="B107" s="85"/>
-      <c r="C107" s="32" t="s">
+      <c r="B107" s="77"/>
+      <c r="C107" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D107" s="6"/>
@@ -5210,10 +5217,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="4"/>
-      <c r="B108" s="85"/>
-      <c r="C108" s="32" t="s">
+      <c r="B108" s="77"/>
+      <c r="C108" s="31" t="s">
         <v>60</v>
       </c>
       <c r="D108" s="6"/>
@@ -5228,10 +5235,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="4"/>
-      <c r="B109" s="85"/>
-      <c r="C109" s="32" t="s">
+      <c r="B109" s="77"/>
+      <c r="C109" s="31" t="s">
         <v>61</v>
       </c>
       <c r="D109" s="6"/>
@@ -5246,10 +5253,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="4"/>
-      <c r="B110" s="85"/>
-      <c r="C110" s="32" t="s">
+      <c r="B110" s="77"/>
+      <c r="C110" s="31" t="s">
         <v>62</v>
       </c>
       <c r="D110" s="6"/>
@@ -5264,10 +5271,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="4"/>
-      <c r="B111" s="85"/>
-      <c r="C111" s="32" t="s">
+      <c r="B111" s="77"/>
+      <c r="C111" s="31" t="s">
         <v>63</v>
       </c>
       <c r="D111" s="6"/>
@@ -5282,10 +5289,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="4"/>
-      <c r="B112" s="85"/>
-      <c r="C112" s="32" t="s">
+      <c r="B112" s="77"/>
+      <c r="C112" s="31" t="s">
         <v>64</v>
       </c>
       <c r="D112" s="6"/>
@@ -5300,10 +5307,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="4"/>
-      <c r="B113" s="85"/>
-      <c r="C113" s="32" t="s">
+      <c r="B113" s="77"/>
+      <c r="C113" s="31" t="s">
         <v>65</v>
       </c>
       <c r="D113" s="6"/>
@@ -5318,10 +5325,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="4"/>
-      <c r="B114" s="85"/>
-      <c r="C114" s="32" t="s">
+      <c r="B114" s="77"/>
+      <c r="C114" s="31" t="s">
         <v>66</v>
       </c>
       <c r="D114" s="6"/>
@@ -5336,12 +5343,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="71" t="s">
+    <row r="115" spans="1:7" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B115" s="85"/>
-      <c r="C115" s="32" t="s">
+      <c r="B115" s="77"/>
+      <c r="C115" s="31" t="s">
         <v>68</v>
       </c>
       <c r="D115" s="6"/>
@@ -5356,10 +5363,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="71"/>
-      <c r="B116" s="85"/>
-      <c r="C116" s="32" t="s">
+    <row r="116" spans="1:7" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="88"/>
+      <c r="B116" s="77"/>
+      <c r="C116" s="31" t="s">
         <v>69</v>
       </c>
       <c r="D116" s="6"/>
@@ -5374,10 +5381,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="71"/>
-      <c r="B117" s="85"/>
-      <c r="C117" s="32" t="s">
+    <row r="117" spans="1:7" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="88"/>
+      <c r="B117" s="77"/>
+      <c r="C117" s="31" t="s">
         <v>70</v>
       </c>
       <c r="D117" s="6"/>
@@ -5392,10 +5399,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="71"/>
-      <c r="B118" s="85"/>
-      <c r="C118" s="37" t="s">
+    <row r="118" spans="1:7" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="88"/>
+      <c r="B118" s="77"/>
+      <c r="C118" s="36" t="s">
         <v>71</v>
       </c>
       <c r="D118" s="6" t="s">
@@ -5412,17 +5419,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="38" t="s">
+    <row r="119" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B119" s="39" t="s">
+      <c r="B119" s="38" t="s">
         <v>74</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D119" s="40" t="s">
+      <c r="D119" s="39" t="s">
         <v>76</v>
       </c>
       <c r="E119" s="7" t="str">
@@ -5436,82 +5443,68 @@
         <v>78</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D120" s="41"/>
-    </row>
-    <row r="122" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D122" s="41"/>
-    </row>
-    <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D124" s="41"/>
-    </row>
-    <row r="126" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D126" s="41"/>
-    </row>
-    <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D128" s="41"/>
-    </row>
-    <row r="130" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D130" s="41"/>
-    </row>
-    <row r="132" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D132" s="41"/>
-    </row>
-    <row r="134" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D134" s="41"/>
-    </row>
-    <row r="136" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D136" s="41"/>
-    </row>
-    <row r="138" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D138" s="41"/>
-    </row>
-    <row r="140" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D140" s="41"/>
-    </row>
-    <row r="145" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D145" s="41"/>
-    </row>
-    <row r="183" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D183" s="41"/>
-    </row>
-    <row r="209" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D209" s="41"/>
-    </row>
-    <row r="282" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D282" s="41"/>
-    </row>
-    <row r="286" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D286" s="41"/>
-    </row>
-    <row r="295" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D295" s="41"/>
-    </row>
-    <row r="297" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D297" s="41"/>
-    </row>
-    <row r="301" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D301" s="41" t="s">
+    <row r="120" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D120" s="40"/>
+    </row>
+    <row r="122" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D122" s="40"/>
+    </row>
+    <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D124" s="40"/>
+    </row>
+    <row r="126" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D126" s="40"/>
+    </row>
+    <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D128" s="40"/>
+    </row>
+    <row r="130" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D130" s="40"/>
+    </row>
+    <row r="132" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D132" s="40"/>
+    </row>
+    <row r="134" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D134" s="40"/>
+    </row>
+    <row r="136" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D136" s="40"/>
+    </row>
+    <row r="138" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D138" s="40"/>
+    </row>
+    <row r="140" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D140" s="40"/>
+    </row>
+    <row r="145" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D145" s="40"/>
+    </row>
+    <row r="183" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D183" s="40"/>
+    </row>
+    <row r="209" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D209" s="40"/>
+    </row>
+    <row r="282" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D282" s="40"/>
+    </row>
+    <row r="286" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D286" s="40"/>
+    </row>
+    <row r="295" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D295" s="40"/>
+    </row>
+    <row r="297" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D297" s="40"/>
+    </row>
+    <row r="301" spans="4:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D301" s="40" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G119"/>
+  <autoFilter ref="A1:G119" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="30">
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="B106:B118"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B66:B69"/>
     <mergeCell ref="A2:A97"/>
     <mergeCell ref="A98:A105"/>
     <mergeCell ref="A115:A118"/>
@@ -5528,6 +5521,20 @@
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="B42:B45"/>
     <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="B106:B118"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="B98:B101"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="E26">
@@ -5910,12 +5917,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E119">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E119" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"正常,异常"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D119" r:id="rId1"/>
+    <hyperlink ref="D119" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId2"/>
@@ -5924,52 +5931,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:IV6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="14.19921875" customWidth="1"/>
-    <col min="3" max="3" width="20.09765625" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" customWidth="1"/>
-    <col min="5" max="5" width="38.19921875" customWidth="1"/>
+    <col min="2" max="2" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="5" max="5" width="38.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="91"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
-    </row>
-    <row r="4" spans="1:5" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="98"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="100"/>
+    </row>
+    <row r="4" spans="1:5" ht="102.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="101"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="103"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="94" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5987,7 +5994,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75.599999999999994" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.15">
       <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
@@ -6001,7 +6008,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="33.75" x14ac:dyDescent="0.15">
       <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
@@ -6015,7 +6022,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.15">
       <c r="B10" s="13" t="s">
         <v>13</v>
       </c>
@@ -6029,7 +6036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.15">
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
@@ -6043,8 +6050,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="88" t="s">
+    <row r="14" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="94" t="s">
         <v>92</v>
       </c>
     </row>
@@ -6062,7 +6069,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="13" t="s">
         <v>39</v>
       </c>
@@ -6076,7 +6083,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="108" hidden="1" x14ac:dyDescent="0.15">
       <c r="B17" s="13" t="s">
         <v>94</v>
       </c>
@@ -6090,7 +6097,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="108" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="108" hidden="1" x14ac:dyDescent="0.15">
       <c r="B18" s="13" t="s">
         <v>97</v>
       </c>
@@ -6104,7 +6111,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="13" t="s">
         <v>42</v>
       </c>
@@ -6118,7 +6125,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="13" t="s">
         <v>45</v>
       </c>
@@ -6132,7 +6139,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="48.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="48.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
         <v>103</v>
       </c>
@@ -6146,54 +6153,54 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:5" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:5" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:5" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="2:5" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="2:5" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="2:5" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="2:5" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="33" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="36" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="37" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="40" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="41" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="42" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="43" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="44" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="45" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="47" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="48" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="49" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="53" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="56" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="57" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="60" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D82" s="22"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D83" s="22"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D114" s="22"/>
     </row>
-    <row r="115" spans="4:4" ht="46.8" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:4" ht="42.75" x14ac:dyDescent="0.15">
       <c r="D115" s="22" t="s">
         <v>105</v>
       </c>
@@ -6212,25 +6219,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" customWidth="1"/>
-    <col min="2" max="2" width="25.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.69921875" customWidth="1"/>
-    <col min="4" max="4" width="43.19921875" customWidth="1"/>
-    <col min="5" max="5" width="17.59765625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="4" max="4" width="43.25" customWidth="1"/>
+    <col min="5" max="5" width="17.625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="18.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6253,24 +6260,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="90.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="49" t="s">
         <v>125</v>
       </c>
       <c r="E2" s="7" t="str">
         <f>IF(ISERROR(SEARCH("norowsselected",D2)),"异常","正常")</f>
         <v>异常</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="61" t="s">
         <v>144</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -6296,7 +6303,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"正常,异常"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6306,14 +6313,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>